<commit_message>
Commit test case changes
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCase/VDS/TestCase_VDS_Transfer Route.xlsx
+++ b/src/main/resources/TestCase/VDS/TestCase_VDS_Transfer Route.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="137">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -344,85 +344,94 @@
     <t>EditValue</t>
   </si>
   <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC004_DS.EditValue</t>
+  </si>
+  <si>
+    <t>//*[@id="row"]/tbody</t>
+  </si>
+  <si>
+    <t>TS22</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>HeaderValue</t>
+  </si>
+  <si>
+    <t>R0005</t>
+  </si>
+  <si>
+    <t>dynamicTableEdit</t>
+  </si>
+  <si>
+    <t>TS23</t>
+  </si>
+  <si>
+    <t>TS24</t>
+  </si>
+  <si>
+    <t>Meilian</t>
+  </si>
+  <si>
+    <t>TC004_DS.PreferredVLSP</t>
+  </si>
+  <si>
+    <t>TC004_DS.PreferredMode</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>CheckApproval</t>
+  </si>
+  <si>
+    <t>SelectCheckBox</t>
+  </si>
+  <si>
+    <t>SaveApprove</t>
+  </si>
+  <si>
+    <t>TS25</t>
+  </si>
+  <si>
+    <t>//*[@id="allbox"]</t>
+  </si>
+  <si>
+    <t>//*[@id="disablebutton"]/a[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="listDiv"]/a[5]/u</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>TS26</t>
+  </si>
+  <si>
+    <t>TS27</t>
+  </si>
+  <si>
+    <t>TS28</t>
+  </si>
+  <si>
     <t>R0006</t>
   </si>
   <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>TC004_DS.EditValue</t>
-  </si>
-  <si>
-    <t>//*[@id="row"]/tbody</t>
-  </si>
-  <si>
-    <t>TS22</t>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>HeaderValue</t>
-  </si>
-  <si>
-    <t>R0005</t>
-  </si>
-  <si>
-    <t>dynamicTableEdit</t>
-  </si>
-  <si>
-    <t>TS23</t>
-  </si>
-  <si>
-    <t>TS24</t>
-  </si>
-  <si>
-    <t>Meilian</t>
-  </si>
-  <si>
-    <t>TC004_DS.PreferredVLSP</t>
-  </si>
-  <si>
-    <t>TC004_DS.PreferredMode</t>
-  </si>
-  <si>
-    <t>Approval</t>
-  </si>
-  <si>
-    <t>Approve</t>
-  </si>
-  <si>
-    <t>CheckApproval</t>
-  </si>
-  <si>
-    <t>SelectCheckBox</t>
-  </si>
-  <si>
-    <t>SaveApprove</t>
-  </si>
-  <si>
-    <t>TS25</t>
-  </si>
-  <si>
-    <t>//*[@id="allbox"]</t>
-  </si>
-  <si>
-    <t>//*[@id="disablebutton"]/a[1]</t>
-  </si>
-  <si>
-    <t>//*[@id="listDiv"]/a[5]/u</t>
-  </si>
-  <si>
-    <t>TC005</t>
-  </si>
-  <si>
-    <t>TS26</t>
-  </si>
-  <si>
-    <t>TS27</t>
-  </si>
-  <si>
-    <t>TS28</t>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>MainMenu</t>
+  </si>
+  <si>
+    <t>Screen</t>
   </si>
 </sst>
 </file>
@@ -813,8 +822,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="146" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -855,7 +864,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -992,7 +1001,9 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
@@ -1000,7 +1011,7 @@
         <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>43</v>
@@ -1021,7 +1032,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>67</v>
@@ -1035,7 +1046,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>40</v>
@@ -1044,7 +1055,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>68</v>
@@ -1067,7 +1078,7 @@
         <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>69</v>
@@ -1090,7 +1101,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>70</v>
@@ -1113,7 +1124,7 @@
         <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>71</v>
@@ -1136,7 +1147,7 @@
         <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>72</v>
@@ -1159,7 +1170,7 @@
         <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>74</v>
@@ -1180,7 +1191,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>100</v>
@@ -1203,7 +1214,7 @@
         <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>54</v>
@@ -1224,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>56</v>
@@ -1240,29 +1251,29 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1271,10 +1282,10 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>71</v>
@@ -1284,7 +1295,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1294,10 +1305,10 @@
         <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>72</v>
@@ -1307,7 +1318,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I21" s="1"/>
     </row>
@@ -1317,10 +1328,10 @@
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>54</v>
@@ -1334,19 +1345,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>9</v>
@@ -1358,16 +1369,16 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>122</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>9</v>
@@ -1379,16 +1390,16 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>9</v>
@@ -1408,8 +1419,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1519,8 +1530,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>42</v>
+      <c r="A8" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>43</v>
@@ -1533,8 +1544,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>42</v>
+      <c r="A9" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>67</v>
@@ -1547,8 +1558,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>42</v>
+      <c r="A10" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>68</v>
@@ -1561,8 +1572,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>42</v>
+      <c r="A11" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>69</v>
@@ -1575,8 +1586,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>42</v>
+      <c r="A12" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>70</v>
@@ -1589,8 +1600,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>42</v>
+      <c r="A13" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>71</v>
@@ -1603,8 +1614,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>42</v>
+      <c r="A14" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>72</v>
@@ -1617,8 +1628,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>42</v>
+      <c r="A15" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>74</v>
@@ -1631,8 +1642,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>42</v>
+      <c r="A16" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>100</v>
@@ -1645,8 +1656,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>42</v>
+      <c r="A17" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>54</v>
@@ -1659,8 +1670,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>42</v>
+      <c r="A18" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>56</v>
@@ -1673,59 +1684,59 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>42</v>
+      <c r="A19" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1843,7 +1854,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1869,13 +1880,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>
@@ -1889,7 +1900,7 @@
         <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
         <v>61</v>

</xml_diff>